<commit_message>
Removed Mahesh and Krishna Sir's 2nd year labs
</commit_message>
<xml_diff>
--- a/Faculty Time Table-CSE,IT.xlsx
+++ b/Faculty Time Table-CSE,IT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="234">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -171,9 +171,6 @@
     <t xml:space="preserve">ECSE-1E</t>
   </si>
   <si>
-    <t xml:space="preserve">C++ LAB-IT-2(B1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">PPS LAB-1D (B2)</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t xml:space="preserve">Mr. Mahesh </t>
   </si>
   <si>
-    <t xml:space="preserve">DS LAB-IT-2  (B1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dr. Masood Ahmed</t>
   </si>
   <si>
@@ -408,7 +402,7 @@
     <t xml:space="preserve">Ms. Vineela</t>
   </si>
   <si>
-    <t xml:space="preserve">C++ LAB - IT-2 (B1)</t>
+    <t xml:space="preserve">C++ LAB-IT-2 (B1)</t>
   </si>
   <si>
     <t xml:space="preserve">OOPC-IT-2</t>
@@ -1215,8 +1209,8 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H156" activeCellId="2" sqref="B95 G90 H156"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A160" activeCellId="0" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2484,9 +2478,7 @@
       <c r="A64" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="17" t="s">
-        <v>48</v>
-      </c>
+      <c r="B64" s="17"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
       <c r="F64" s="19"/>
@@ -2513,14 +2505,14 @@
         <v>20</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
       <c r="E65" s="18"/>
       <c r="F65" s="19"/>
       <c r="G65" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H65" s="17"/>
       <c r="I65" s="18"/>
@@ -2551,7 +2543,7 @@
       <c r="F66" s="19"/>
       <c r="G66" s="21"/>
       <c r="H66" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I66" s="17"/>
       <c r="J66" s="18"/>
@@ -2573,7 +2565,7 @@
       </c>
       <c r="B67" s="17"/>
       <c r="C67" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D67" s="17"/>
       <c r="E67" s="17"/>
@@ -2648,7 +2640,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -2720,7 +2712,7 @@
       </c>
       <c r="B72" s="17"/>
       <c r="C72" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E72" s="18"/>
       <c r="F72" s="19" t="s">
@@ -2728,7 +2720,7 @@
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I72" s="29"/>
       <c r="J72" s="29"/>
@@ -2749,14 +2741,14 @@
         <v>19</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" s="22"/>
       <c r="D73" s="17"/>
       <c r="E73" s="17"/>
       <c r="F73" s="19"/>
       <c r="H73" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I73" s="17"/>
       <c r="J73" s="17"/>
@@ -2778,7 +2770,7 @@
       </c>
       <c r="C74" s="22"/>
       <c r="E74" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F74" s="19"/>
       <c r="G74" s="21"/>
@@ -2802,7 +2794,7 @@
         <v>21</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="17"/>
@@ -2829,12 +2821,12 @@
         <v>22</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C76" s="17"/>
       <c r="D76" s="18"/>
       <c r="E76" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F76" s="19"/>
       <c r="H76" s="17"/>
@@ -2892,7 +2884,7 @@
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -2950,11 +2942,11 @@
         <v>17</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J81" s="17"/>
       <c r="K81" s="10"/>
@@ -2964,14 +2956,14 @@
         <v>19</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C82" s="17"/>
       <c r="D82" s="17"/>
       <c r="F82" s="19"/>
       <c r="G82" s="22"/>
       <c r="H82" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I82" s="17"/>
       <c r="J82" s="17"/>
@@ -2982,13 +2974,13 @@
         <v>20</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C83" s="17"/>
       <c r="E83" s="17"/>
       <c r="F83" s="19"/>
       <c r="G83" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H83" s="29"/>
       <c r="I83" s="17"/>
@@ -3007,7 +2999,7 @@
       <c r="G84" s="17"/>
       <c r="H84" s="18"/>
       <c r="I84" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J84" s="17"/>
       <c r="K84" s="10"/>
@@ -3017,7 +3009,7 @@
         <v>22</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C85" s="17" t="s">
         <v>18</v>
@@ -3026,7 +3018,7 @@
       <c r="E85" s="17"/>
       <c r="F85" s="19"/>
       <c r="G85" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H85" s="17"/>
       <c r="J85" s="18"/>
@@ -3062,7 +3054,7 @@
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3133,7 +3125,7 @@
         <v>15</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C90" s="17"/>
       <c r="D90" s="17"/>
@@ -3142,7 +3134,7 @@
         <v>17</v>
       </c>
       <c r="G90" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
@@ -3165,17 +3157,17 @@
       </c>
       <c r="B91" s="17"/>
       <c r="C91" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="17"/>
       <c r="F91" s="19"/>
       <c r="G91" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H91" s="17"/>
       <c r="I91" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J91" s="17"/>
       <c r="K91" s="10"/>
@@ -3195,7 +3187,7 @@
         <v>20</v>
       </c>
       <c r="B92" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C92" s="17"/>
       <c r="D92" s="17"/>
@@ -3203,7 +3195,7 @@
       <c r="F92" s="19"/>
       <c r="G92" s="17"/>
       <c r="H92" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I92" s="17"/>
       <c r="J92" s="17"/>
@@ -3224,14 +3216,14 @@
         <v>21</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C93" s="17"/>
       <c r="D93" s="17"/>
       <c r="E93" s="17"/>
       <c r="F93" s="19"/>
       <c r="G93" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
@@ -3254,16 +3246,16 @@
       </c>
       <c r="B94" s="17"/>
       <c r="C94" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F94" s="19"/>
       <c r="G94" s="17"/>
       <c r="H94" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I94" s="17"/>
       <c r="J94" s="17"/>
@@ -3284,7 +3276,7 @@
         <v>23</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C95" s="17"/>
       <c r="D95" s="17"/>
@@ -3331,7 +3323,7 @@
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -3401,9 +3393,7 @@
         <v>15</v>
       </c>
       <c r="B99" s="17"/>
-      <c r="C99" s="17" t="s">
-        <v>76</v>
-      </c>
+      <c r="C99" s="17"/>
       <c r="D99" s="17"/>
       <c r="E99" s="17"/>
       <c r="F99" s="19" t="s">
@@ -3568,7 +3558,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
@@ -3637,7 +3627,7 @@
         <v>15</v>
       </c>
       <c r="B108" s="32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C108" s="32"/>
       <c r="D108" s="32"/>
@@ -3665,7 +3655,7 @@
         <v>19</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C109" s="32"/>
       <c r="D109" s="32"/>
@@ -3796,7 +3786,7 @@
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
@@ -3845,7 +3835,7 @@
         <v>15</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C117" s="17"/>
       <c r="D117" s="17"/>
@@ -3855,7 +3845,7 @@
       </c>
       <c r="G117" s="17"/>
       <c r="H117" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I117" s="17"/>
       <c r="J117" s="17"/>
@@ -3866,17 +3856,17 @@
       </c>
       <c r="B118" s="17"/>
       <c r="C118" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D118" s="17"/>
       <c r="E118" s="17"/>
       <c r="F118" s="19"/>
       <c r="G118" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H118" s="17"/>
       <c r="I118" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J118" s="17"/>
     </row>
@@ -3885,17 +3875,17 @@
         <v>20</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C119" s="17"/>
       <c r="D119" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E119" s="17"/>
       <c r="F119" s="19"/>
       <c r="G119" s="17"/>
       <c r="H119" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I119" s="17"/>
       <c r="J119" s="17"/>
@@ -3905,13 +3895,13 @@
         <v>21</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C120" s="17"/>
       <c r="D120" s="17"/>
       <c r="F120" s="19"/>
       <c r="G120" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H120" s="17"/>
       <c r="I120" s="17"/>
@@ -3922,17 +3912,17 @@
         <v>22</v>
       </c>
       <c r="B121" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C121" s="17"/>
       <c r="D121" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E121" s="17"/>
       <c r="F121" s="19"/>
       <c r="G121" s="17"/>
       <c r="H121" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I121" s="17"/>
       <c r="J121" s="17"/>
@@ -3942,7 +3932,7 @@
         <v>23</v>
       </c>
       <c r="B122" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C122" s="17"/>
       <c r="D122" s="17"/>
@@ -3967,7 +3957,7 @@
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -4016,18 +4006,18 @@
         <v>15</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C126" s="17"/>
       <c r="D126" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E126" s="17"/>
       <c r="F126" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G126" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
@@ -4038,7 +4028,7 @@
         <v>19</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C127" s="17"/>
       <c r="D127" s="17"/>
@@ -4046,7 +4036,7 @@
       <c r="F127" s="19"/>
       <c r="G127" s="17"/>
       <c r="H127" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I127" s="17"/>
       <c r="J127" s="17"/>
@@ -4057,7 +4047,7 @@
       </c>
       <c r="B128" s="17"/>
       <c r="C128" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D128" s="17"/>
       <c r="E128" s="17"/>
@@ -4073,13 +4063,13 @@
       </c>
       <c r="B129" s="17"/>
       <c r="C129" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D129" s="17"/>
       <c r="E129" s="17"/>
       <c r="F129" s="19"/>
       <c r="G129" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H129" s="17"/>
       <c r="I129" s="17"/>
@@ -4090,7 +4080,7 @@
         <v>22</v>
       </c>
       <c r="B130" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C130" s="17"/>
       <c r="D130" s="17"/>
@@ -4108,7 +4098,7 @@
       <c r="B131" s="17"/>
       <c r="C131" s="17"/>
       <c r="D131" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E131" s="17"/>
       <c r="F131" s="19"/>
@@ -4131,7 +4121,7 @@
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="13"/>
@@ -4201,7 +4191,7 @@
       </c>
       <c r="B135" s="17"/>
       <c r="D135" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F135" s="19" t="s">
         <v>17</v>
@@ -4230,7 +4220,7 @@
       <c r="E136" s="24"/>
       <c r="F136" s="19"/>
       <c r="G136" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
@@ -4251,14 +4241,14 @@
         <v>20</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C137" s="17"/>
       <c r="D137" s="17"/>
       <c r="E137" s="17"/>
       <c r="F137" s="19"/>
       <c r="G137" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H137" s="22"/>
       <c r="I137" s="17"/>
@@ -4279,7 +4269,7 @@
         <v>21</v>
       </c>
       <c r="B138" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C138" s="17"/>
       <c r="D138" s="17"/>
@@ -4287,11 +4277,11 @@
       <c r="F138" s="19"/>
       <c r="G138" s="17"/>
       <c r="H138" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I138" s="24"/>
       <c r="J138" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L138" s="0"/>
       <c r="M138" s="0"/>
@@ -4315,7 +4305,7 @@
       <c r="F139" s="19"/>
       <c r="G139" s="17"/>
       <c r="H139" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I139" s="17"/>
       <c r="J139" s="22"/>
@@ -4378,7 +4368,7 @@
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B142" s="13"/>
       <c r="C142" s="13"/>
@@ -4454,7 +4444,7 @@
         <v>17</v>
       </c>
       <c r="G144" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H144" s="17"/>
       <c r="I144" s="17"/>
@@ -4604,7 +4594,7 @@
     </row>
     <row r="151" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B151" s="13"/>
       <c r="C151" s="13"/>
@@ -4655,7 +4645,7 @@
       </c>
       <c r="B153" s="17"/>
       <c r="C153" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D153" s="32"/>
       <c r="E153" s="32"/>
@@ -4701,7 +4691,7 @@
         <v>21</v>
       </c>
       <c r="B156" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C156" s="32"/>
       <c r="D156" s="32"/>
@@ -4745,7 +4735,7 @@
     <row r="159" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="160" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
@@ -4812,7 +4802,7 @@
         <v>19</v>
       </c>
       <c r="B163" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C163" s="21"/>
       <c r="D163" s="21"/>
@@ -4841,7 +4831,7 @@
         <v>21</v>
       </c>
       <c r="B165" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C165" s="35"/>
       <c r="D165" s="35"/>
@@ -4884,7 +4874,7 @@
     <row r="168" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B169" s="13"/>
       <c r="C169" s="13"/>
@@ -4935,7 +4925,7 @@
         <v>15</v>
       </c>
       <c r="B171" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C171" s="17"/>
       <c r="D171" s="17"/>
@@ -4967,7 +4957,7 @@
         <v>20</v>
       </c>
       <c r="B173" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C173" s="35"/>
       <c r="D173" s="35"/>
@@ -4976,7 +4966,7 @@
       <c r="G173" s="17"/>
       <c r="H173" s="17"/>
       <c r="I173" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J173" s="17"/>
       <c r="L173" s="1"/>
@@ -5038,7 +5028,7 @@
     </row>
     <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B178" s="13"/>
       <c r="C178" s="13"/>
@@ -5089,7 +5079,7 @@
         <v>15</v>
       </c>
       <c r="B180" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C180" s="17"/>
       <c r="D180" s="17"/>
@@ -5098,11 +5088,11 @@
         <v>17</v>
       </c>
       <c r="G180" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H180" s="17"/>
       <c r="J180" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="181" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5110,17 +5100,17 @@
         <v>19</v>
       </c>
       <c r="B181" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C181" s="17"/>
       <c r="D181" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E181" s="17"/>
       <c r="F181" s="19"/>
       <c r="G181" s="18"/>
       <c r="H181" s="36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I181" s="36"/>
       <c r="J181" s="22"/>
@@ -5131,13 +5121,13 @@
       </c>
       <c r="B182" s="17"/>
       <c r="C182" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D182" s="17"/>
       <c r="E182" s="22"/>
       <c r="F182" s="19"/>
       <c r="G182" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I182" s="17"/>
       <c r="J182" s="17"/>
@@ -5148,17 +5138,17 @@
       </c>
       <c r="B183" s="17"/>
       <c r="C183" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D183" s="17"/>
       <c r="E183" s="22"/>
       <c r="F183" s="19"/>
       <c r="G183" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H183" s="22"/>
       <c r="I183" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J183" s="17"/>
     </row>
@@ -5167,17 +5157,17 @@
         <v>22</v>
       </c>
       <c r="B184" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C184" s="17"/>
       <c r="D184" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E184" s="17"/>
       <c r="F184" s="19"/>
       <c r="G184" s="22"/>
       <c r="H184" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I184" s="17"/>
       <c r="J184" s="22"/>
@@ -5210,7 +5200,7 @@
     </row>
     <row r="187" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B187" s="13"/>
       <c r="C187" s="13"/>
@@ -5319,7 +5309,7 @@
         <v>22</v>
       </c>
       <c r="B193" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C193" s="17"/>
       <c r="D193" s="17"/>
@@ -5358,7 +5348,7 @@
     </row>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B196" s="13"/>
       <c r="C196" s="13"/>
@@ -5425,7 +5415,7 @@
         <v>19</v>
       </c>
       <c r="B199" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C199" s="29"/>
       <c r="D199" s="29"/>
@@ -5447,7 +5437,7 @@
       <c r="F200" s="19"/>
       <c r="G200" s="17"/>
       <c r="H200" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I200" s="18"/>
       <c r="J200" s="22"/>
@@ -5463,7 +5453,7 @@
       <c r="E201" s="22"/>
       <c r="F201" s="19"/>
       <c r="G201" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H201" s="17"/>
       <c r="I201" s="17"/>
@@ -5480,7 +5470,7 @@
       <c r="E202" s="17"/>
       <c r="F202" s="19"/>
       <c r="G202" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H202" s="29"/>
       <c r="I202" s="17"/>
@@ -5493,7 +5483,7 @@
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
       <c r="D203" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E203" s="29"/>
       <c r="F203" s="19"/>
@@ -5516,7 +5506,7 @@
     </row>
     <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B205" s="13"/>
       <c r="C205" s="13"/>
@@ -5568,18 +5558,18 @@
       </c>
       <c r="B207" s="17"/>
       <c r="C207" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D207" s="17"/>
       <c r="E207" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F207" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G207" s="17"/>
       <c r="H207" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I207" s="17"/>
       <c r="J207" s="17"/>
@@ -5590,14 +5580,14 @@
       </c>
       <c r="B208" s="17"/>
       <c r="C208" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D208" s="17"/>
       <c r="E208" s="17"/>
       <c r="F208" s="19"/>
       <c r="G208" s="17"/>
       <c r="H208" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I208" s="17"/>
       <c r="J208" s="17"/>
@@ -5607,7 +5597,7 @@
         <v>20</v>
       </c>
       <c r="B209" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C209" s="17"/>
       <c r="D209" s="17"/>
@@ -5616,7 +5606,7 @@
       <c r="G209" s="17"/>
       <c r="H209" s="17"/>
       <c r="I209" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J209" s="17"/>
       <c r="L209" s="1"/>
@@ -5627,13 +5617,13 @@
       </c>
       <c r="B210" s="17"/>
       <c r="C210" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D210" s="17"/>
       <c r="E210" s="17"/>
       <c r="F210" s="19"/>
       <c r="G210" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H210" s="17"/>
       <c r="I210" s="17"/>
@@ -5647,13 +5637,13 @@
       <c r="B211" s="17"/>
       <c r="C211" s="17"/>
       <c r="D211" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E211" s="22"/>
       <c r="F211" s="19"/>
       <c r="G211" s="17"/>
       <c r="H211" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I211" s="17"/>
       <c r="J211" s="17"/>
@@ -6009,7 +5999,7 @@
   <dimension ref="B1:Z91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="2" sqref="B95 G90 G12"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="1" sqref="A160 G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6067,7 +6057,7 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -6097,7 +6087,7 @@
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -6161,7 +6151,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -6170,7 +6160,7 @@
         <v>17</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -6194,14 +6184,14 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="19"/>
       <c r="I9" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -6225,14 +6215,14 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="19"/>
       <c r="I10" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -6258,14 +6248,14 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="19"/>
       <c r="I11" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
@@ -6289,14 +6279,14 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="19"/>
       <c r="I12" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
@@ -6343,7 +6333,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -6408,7 +6398,7 @@
       <c r="C16" s="15"/>
       <c r="D16" s="41"/>
       <c r="E16" s="41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" s="41"/>
       <c r="G16" s="41"/>
@@ -6417,7 +6407,7 @@
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
@@ -6429,14 +6419,14 @@
       <c r="C17" s="15"/>
       <c r="D17" s="41"/>
       <c r="E17" s="41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F17" s="41"/>
       <c r="G17" s="41"/>
       <c r="H17" s="19"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
@@ -6448,14 +6438,14 @@
       <c r="C18" s="15"/>
       <c r="D18" s="41"/>
       <c r="E18" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="19"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
@@ -6467,14 +6457,14 @@
       <c r="C19" s="15"/>
       <c r="D19" s="41"/>
       <c r="E19" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="19"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
@@ -6486,14 +6476,14 @@
       <c r="C20" s="15"/>
       <c r="D20" s="41"/>
       <c r="E20" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="19"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
@@ -6515,7 +6505,7 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -6568,7 +6558,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -6577,7 +6567,7 @@
       </c>
       <c r="I24" s="17"/>
       <c r="J24" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
@@ -6589,14 +6579,14 @@
       <c r="C25" s="15"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
       <c r="H25" s="19"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
@@ -6608,14 +6598,14 @@
       <c r="C26" s="15"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="19"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
@@ -6627,14 +6617,14 @@
       <c r="C27" s="15"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="19"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
@@ -6646,14 +6636,14 @@
       <c r="C28" s="15"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="H28" s="19"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
@@ -6701,7 +6691,7 @@
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -6753,7 +6743,7 @@
       </c>
       <c r="C34" s="15"/>
       <c r="E34" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
@@ -6762,7 +6752,7 @@
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
@@ -6779,7 +6769,7 @@
       <c r="H35" s="19"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
@@ -6791,13 +6781,13 @@
       <c r="C36" s="15"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
       <c r="H36" s="19"/>
       <c r="I36" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
@@ -6810,14 +6800,14 @@
       <c r="C37" s="15"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
       <c r="H37" s="19"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
@@ -6828,14 +6818,14 @@
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
       <c r="H38" s="19"/>
       <c r="I38" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -6858,7 +6848,7 @@
     </row>
     <row r="40" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -6911,7 +6901,7 @@
       <c r="C42" s="15"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
@@ -6920,7 +6910,7 @@
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
@@ -6932,14 +6922,14 @@
       <c r="C43" s="15"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
       <c r="H43" s="19"/>
       <c r="I43" s="17"/>
       <c r="J43" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
@@ -6951,14 +6941,14 @@
       <c r="C44" s="15"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
       <c r="H44" s="19"/>
       <c r="I44" s="17"/>
       <c r="J44" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
@@ -6970,14 +6960,14 @@
       <c r="C45" s="15"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
       <c r="H45" s="19"/>
       <c r="I45" s="17"/>
       <c r="J45" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
@@ -6989,14 +6979,14 @@
       <c r="C46" s="15"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
       <c r="H46" s="19"/>
       <c r="I46" s="17"/>
       <c r="J46" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
@@ -7018,7 +7008,7 @@
     </row>
     <row r="48" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -7070,7 +7060,7 @@
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
@@ -7089,14 +7079,14 @@
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
       <c r="H51" s="19"/>
       <c r="I51" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J51" s="17"/>
       <c r="K51" s="18"/>
@@ -7138,7 +7128,7 @@
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
@@ -7157,7 +7147,7 @@
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
       <c r="F55" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="19"/>
@@ -7168,7 +7158,7 @@
     </row>
     <row r="57" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -7220,7 +7210,7 @@
       </c>
       <c r="C59" s="15"/>
       <c r="E59" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
@@ -7229,7 +7219,7 @@
       </c>
       <c r="I59" s="43"/>
       <c r="J59" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
@@ -7241,14 +7231,14 @@
       <c r="C60" s="15"/>
       <c r="D60" s="17"/>
       <c r="E60" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
       <c r="H60" s="19"/>
       <c r="I60" s="43"/>
       <c r="J60" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K60" s="17"/>
       <c r="L60" s="17"/>
@@ -7260,14 +7250,14 @@
       <c r="C61" s="15"/>
       <c r="D61" s="17"/>
       <c r="E61" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="17"/>
       <c r="H61" s="19"/>
       <c r="I61" s="43"/>
       <c r="J61" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K61" s="17"/>
       <c r="L61" s="17"/>
@@ -7279,14 +7269,14 @@
       <c r="C62" s="15"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
       <c r="H62" s="19"/>
       <c r="I62" s="43"/>
       <c r="J62" s="17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
@@ -7298,14 +7288,14 @@
       <c r="C63" s="15"/>
       <c r="D63" s="17"/>
       <c r="E63" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="17"/>
       <c r="H63" s="19"/>
       <c r="I63" s="43"/>
       <c r="J63" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K63" s="17"/>
       <c r="L63" s="17"/>
@@ -7327,7 +7317,7 @@
     </row>
     <row r="66" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
@@ -7379,7 +7369,7 @@
       </c>
       <c r="C68" s="15"/>
       <c r="E68" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="17"/>
@@ -7388,7 +7378,7 @@
       </c>
       <c r="I68" s="43"/>
       <c r="J68" s="17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
@@ -7400,14 +7390,14 @@
       <c r="C69" s="15"/>
       <c r="D69" s="17"/>
       <c r="E69" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="17"/>
       <c r="H69" s="19"/>
       <c r="I69" s="43"/>
       <c r="J69" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K69" s="17"/>
       <c r="L69" s="17"/>
@@ -7419,14 +7409,14 @@
       <c r="C70" s="15"/>
       <c r="D70" s="17"/>
       <c r="E70" s="17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="17"/>
       <c r="H70" s="19"/>
       <c r="I70" s="43"/>
       <c r="J70" s="17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K70" s="17"/>
       <c r="L70" s="17"/>
@@ -7438,14 +7428,14 @@
       <c r="C71" s="15"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
       <c r="H71" s="19"/>
       <c r="I71" s="43"/>
       <c r="J71" s="17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K71" s="17"/>
       <c r="L71" s="17"/>
@@ -7457,14 +7447,14 @@
       <c r="C72" s="15"/>
       <c r="D72" s="17"/>
       <c r="E72" s="17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="17"/>
       <c r="H72" s="19"/>
       <c r="I72" s="43"/>
       <c r="J72" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K72" s="17"/>
       <c r="L72" s="17"/>
@@ -7486,7 +7476,7 @@
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
@@ -7538,7 +7528,7 @@
       </c>
       <c r="C77" s="15"/>
       <c r="E77" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="17"/>
@@ -7547,7 +7537,7 @@
       </c>
       <c r="I77" s="17"/>
       <c r="J77" s="17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K77" s="17"/>
       <c r="L77" s="17"/>
@@ -7559,14 +7549,14 @@
       <c r="C78" s="15"/>
       <c r="D78" s="17"/>
       <c r="E78" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="17"/>
       <c r="H78" s="19"/>
       <c r="I78" s="17"/>
       <c r="J78" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K78" s="17"/>
       <c r="L78" s="17"/>
@@ -7578,14 +7568,14 @@
       <c r="C79" s="15"/>
       <c r="D79" s="17"/>
       <c r="E79" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
       <c r="H79" s="19"/>
       <c r="I79" s="17"/>
       <c r="J79" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K79" s="17"/>
       <c r="L79" s="17"/>
@@ -7597,14 +7587,14 @@
       <c r="C80" s="15"/>
       <c r="D80" s="17"/>
       <c r="E80" s="17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="17"/>
       <c r="H80" s="19"/>
       <c r="I80" s="17"/>
       <c r="J80" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K80" s="17"/>
       <c r="L80" s="17"/>
@@ -7616,14 +7606,14 @@
       <c r="C81" s="15"/>
       <c r="D81" s="17"/>
       <c r="E81" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="17"/>
       <c r="H81" s="19"/>
       <c r="I81" s="17"/>
       <c r="J81" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K81" s="17"/>
       <c r="L81" s="17"/>
@@ -7645,7 +7635,7 @@
     </row>
     <row r="84" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
@@ -7704,7 +7694,7 @@
         <v>17</v>
       </c>
       <c r="I86" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J86" s="17"/>
       <c r="K86" s="17"/>
@@ -7717,13 +7707,13 @@
       <c r="C87" s="15"/>
       <c r="D87" s="17"/>
       <c r="E87" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="17"/>
       <c r="H87" s="19"/>
       <c r="I87" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J87" s="17"/>
       <c r="K87" s="17"/>
@@ -7740,7 +7730,7 @@
       <c r="G88" s="17"/>
       <c r="H88" s="19"/>
       <c r="I88" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J88" s="17"/>
       <c r="K88" s="17"/>
@@ -7753,14 +7743,14 @@
       <c r="C89" s="15"/>
       <c r="D89" s="17"/>
       <c r="E89" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="17"/>
       <c r="H89" s="19"/>
       <c r="I89" s="17"/>
       <c r="J89" s="17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
@@ -7772,14 +7762,14 @@
       <c r="C90" s="15"/>
       <c r="D90" s="17"/>
       <c r="E90" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="17"/>
       <c r="H90" s="19"/>
       <c r="I90" s="17"/>
       <c r="J90" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K90" s="17"/>
       <c r="L90" s="17"/>

</xml_diff>

<commit_message>
Lab TT matched with class time table,Removed 3rd and 4th year labs and allocated pending DS Lab(2D)(B1) to A001
</commit_message>
<xml_diff>
--- a/Faculty Time Table-CSE,IT.xlsx
+++ b/Faculty Time Table-CSE,IT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty TT" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="192">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -426,40 +426,13 @@
     <t xml:space="preserve">LAB TIME TABLE - 2022-2023 (I Semester)  </t>
   </si>
   <si>
-    <t xml:space="preserve">A001 (CNS/IS LAB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS 4IT LAB (B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4A LAB (B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4D LAB (B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4B LAB (B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4B LAB (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4C LAB (B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4A LAB (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS 4IT LAB (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4C LAB (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNS 4D LAB (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A110A (ITWS, SE LAB)</t>
+    <t xml:space="preserve">A001 (DS LAB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS LAB- CSE-2D-(B1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A110A (ITWS LAB)</t>
   </si>
   <si>
     <t xml:space="preserve">ITWS LAB – CSE-2D(B2)</t>
@@ -471,58 +444,7 @@
     <t xml:space="preserve">ITWS LAB - IT-2(B2) </t>
   </si>
   <si>
-    <t xml:space="preserve">SE LAB-CSE-3B(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE LAB-CSE-3B(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE LAB-CSE-3A(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE LAB-CSE-3C(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE LAB-CSE-3IT(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE LAB-CSE-3A(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE LAB-CSE-3C(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A110B (CN/DCCN LAB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3B(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3C(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3A(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3D(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3B(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCCN LAB-CSE-3IT(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3C(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSM-3(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSE-3A(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN LAB-CSM-3(B2)</t>
+    <t xml:space="preserve">A110B </t>
   </si>
   <si>
     <t xml:space="preserve">A214A/1 (PPS,DS)</t>
@@ -555,7 +477,7 @@
     <t xml:space="preserve">PPS LAB-CSE-1E(B1)</t>
   </si>
   <si>
-    <t xml:space="preserve">A201B ( ITWS, PYTHON, WP, ML,SE )</t>
+    <t xml:space="preserve">A201B ( ITWS, PYTHON )</t>
   </si>
   <si>
     <t xml:space="preserve">PYTHON LAB - CSM-2(B2)</t>
@@ -567,40 +489,13 @@
     <t xml:space="preserve">PYTHON LAB – CSM-2(B1)</t>
   </si>
   <si>
-    <t xml:space="preserve">WP LAB -IT-3</t>
-  </si>
-  <si>
     <t xml:space="preserve">ITWS LAB - CSE-2D(B1)</t>
   </si>
   <si>
-    <t xml:space="preserve">SE-CSE-3D(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ML LAB - CSM-3(B2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">ITWS LAB – CSE-2B(B2)</t>
   </si>
   <si>
-    <t xml:space="preserve">ML LAB - CSM-3-(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A214D ( ACS LAB-3A,3B,3C,3D, IT-3, CSM-3 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACS LAB-CSE-3C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACS LAB-CSE-3D/IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACS LAB-CSM-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACS LAB-CSE-3B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACS LAB-CSE-3A</t>
+    <t xml:space="preserve">A214D</t>
   </si>
   <si>
     <t xml:space="preserve">A203 ( DS )</t>
@@ -618,7 +513,7 @@
     <t xml:space="preserve">DS LAB- CSE-2A-(B1)</t>
   </si>
   <si>
-    <t xml:space="preserve">DS LAB- CSE-2D-(B1)</t>
+    <t xml:space="preserve">DS LAB- CSE-2D-(B2)</t>
   </si>
   <si>
     <t xml:space="preserve">DS LAB- CSE-2C-(B1)</t>
@@ -669,37 +564,16 @@
     <t xml:space="preserve">C++ LAB- CSE-2C-(B1)</t>
   </si>
   <si>
-    <t xml:space="preserve">A201A ( ITWS,WT )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT-CSE-3B(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT-CSE-3C(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT-CSE-3A(B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT-CSE-3B(B1)</t>
+    <t xml:space="preserve">A201A ( ITWS )</t>
   </si>
   <si>
     <t xml:space="preserve">ITWS-CSE-2A(B2)</t>
   </si>
   <si>
-    <t xml:space="preserve">WT-CSE-3A(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT- IT-2(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT-CSE-3D</t>
+    <t xml:space="preserve">ITWS- IT-2(B1)</t>
   </si>
   <si>
     <t xml:space="preserve">ITWS-CSE-2A(B1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WT-CSE-3C(B1)</t>
   </si>
   <si>
     <t xml:space="preserve">A214A/2 (PPS)</t>
@@ -860,7 +734,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -887,14 +761,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF6D"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAA95"/>
-        <bgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -953,7 +821,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,10 +938,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1082,19 +946,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1116,6 +972,10 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1176,9 +1036,9 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF6D"/>
+      <rgbColor rgb="FFD4EA6B"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFFAA95"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -1209,8 +1069,8 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I228" activeCellId="0" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2719,11 +2579,11 @@
         <v>17</v>
       </c>
       <c r="G72" s="17"/>
-      <c r="H72" s="29" t="s">
+      <c r="H72" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
+      <c r="I72" s="17"/>
+      <c r="J72" s="17"/>
       <c r="K72" s="10"/>
       <c r="L72" s="0"/>
       <c r="M72" s="0"/>
@@ -2825,7 +2685,7 @@
       </c>
       <c r="C76" s="17"/>
       <c r="D76" s="18"/>
-      <c r="E76" s="29" t="s">
+      <c r="E76" s="17" t="s">
         <v>56</v>
       </c>
       <c r="F76" s="19"/>
@@ -2979,10 +2839,10 @@
       <c r="C83" s="17"/>
       <c r="E83" s="17"/>
       <c r="F83" s="19"/>
-      <c r="G83" s="29" t="s">
+      <c r="G83" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="H83" s="29"/>
+      <c r="H83" s="17"/>
       <c r="I83" s="17"/>
       <c r="J83" s="17"/>
       <c r="K83" s="10"/>
@@ -3419,7 +3279,7 @@
         <v>19</v>
       </c>
       <c r="B100" s="17"/>
-      <c r="C100" s="30"/>
+      <c r="C100" s="29"/>
       <c r="D100" s="22"/>
       <c r="E100" s="21"/>
       <c r="F100" s="19"/>
@@ -3444,7 +3304,7 @@
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="22"/>
-      <c r="D101" s="31"/>
+      <c r="D101" s="30"/>
       <c r="E101" s="17"/>
       <c r="F101" s="19"/>
       <c r="G101" s="17"/>
@@ -3626,11 +3486,11 @@
       <c r="A108" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B108" s="32" t="s">
+      <c r="B108" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C108" s="32"/>
-      <c r="D108" s="32"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
       <c r="E108" s="17"/>
       <c r="F108" s="19" t="s">
         <v>17</v>
@@ -3654,11 +3514,11 @@
       <c r="A109" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B109" s="32" t="s">
+      <c r="B109" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="17"/>
       <c r="E109" s="17"/>
       <c r="F109" s="19"/>
       <c r="G109" s="17"/>
@@ -4159,7 +4019,7 @@
       <c r="E134" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F134" s="33" t="s">
+      <c r="F134" s="31" t="s">
         <v>10</v>
       </c>
       <c r="G134" s="16" t="s">
@@ -4190,7 +4050,7 @@
         <v>15</v>
       </c>
       <c r="B135" s="17"/>
-      <c r="D135" s="34" t="s">
+      <c r="D135" s="32" t="s">
         <v>94</v>
       </c>
       <c r="F135" s="19" t="s">
@@ -4219,7 +4079,7 @@
       <c r="D136" s="17"/>
       <c r="E136" s="24"/>
       <c r="F136" s="19"/>
-      <c r="G136" s="29" t="s">
+      <c r="G136" s="17" t="s">
         <v>95</v>
       </c>
       <c r="H136" s="17"/>
@@ -4276,7 +4136,7 @@
       <c r="E138" s="17"/>
       <c r="F138" s="19"/>
       <c r="G138" s="17"/>
-      <c r="H138" s="29" t="s">
+      <c r="H138" s="17" t="s">
         <v>95</v>
       </c>
       <c r="I138" s="24"/>
@@ -4644,11 +4504,11 @@
         <v>15</v>
       </c>
       <c r="B153" s="17"/>
-      <c r="C153" s="32" t="s">
+      <c r="C153" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="D153" s="32"/>
-      <c r="E153" s="32"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
       <c r="F153" s="19" t="s">
         <v>17</v>
       </c>
@@ -4690,11 +4550,11 @@
       <c r="A156" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B156" s="32" t="s">
+      <c r="B156" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C156" s="32"/>
-      <c r="D156" s="32"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="17"/>
       <c r="E156" s="17"/>
       <c r="F156" s="19"/>
       <c r="G156" s="17"/>
@@ -4830,11 +4690,11 @@
       <c r="A165" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B165" s="35" t="s">
+      <c r="B165" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C165" s="35"/>
-      <c r="D165" s="35"/>
+      <c r="C165" s="21"/>
+      <c r="D165" s="21"/>
       <c r="E165" s="17"/>
       <c r="F165" s="19"/>
       <c r="G165" s="21"/>
@@ -4956,11 +4816,11 @@
       <c r="A173" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B173" s="35" t="s">
+      <c r="B173" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C173" s="35"/>
-      <c r="D173" s="35"/>
+      <c r="C173" s="21"/>
+      <c r="D173" s="21"/>
       <c r="E173" s="17"/>
       <c r="F173" s="19"/>
       <c r="G173" s="17"/>
@@ -5109,10 +4969,10 @@
       <c r="E181" s="17"/>
       <c r="F181" s="19"/>
       <c r="G181" s="18"/>
-      <c r="H181" s="36" t="s">
+      <c r="H181" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="I181" s="36"/>
+      <c r="I181" s="33"/>
       <c r="J181" s="22"/>
     </row>
     <row r="182" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5414,11 +5274,11 @@
       <c r="A199" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B199" s="29" t="s">
+      <c r="B199" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C199" s="29"/>
-      <c r="D199" s="29"/>
+      <c r="C199" s="17"/>
+      <c r="D199" s="17"/>
       <c r="E199" s="17"/>
       <c r="F199" s="19"/>
       <c r="G199" s="17"/>
@@ -5436,7 +5296,7 @@
       <c r="E200" s="18"/>
       <c r="F200" s="19"/>
       <c r="G200" s="17"/>
-      <c r="H200" s="29" t="s">
+      <c r="H200" s="17" t="s">
         <v>126</v>
       </c>
       <c r="I200" s="18"/>
@@ -5469,10 +5329,10 @@
       <c r="D202" s="17"/>
       <c r="E202" s="17"/>
       <c r="F202" s="19"/>
-      <c r="G202" s="29" t="s">
+      <c r="G202" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="H202" s="29"/>
+      <c r="H202" s="17"/>
       <c r="I202" s="17"/>
       <c r="J202" s="17"/>
     </row>
@@ -5482,10 +5342,10 @@
       </c>
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
-      <c r="D203" s="29" t="s">
+      <c r="D203" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E203" s="29"/>
+      <c r="E203" s="17"/>
       <c r="F203" s="19"/>
       <c r="G203" s="17"/>
       <c r="H203" s="17"/>
@@ -5998,8 +5858,8 @@
   </sheetPr>
   <dimension ref="B1:Z91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6097,7 +5957,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="37"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6145,164 +6005,146 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="17" t="s">
-        <v>134</v>
-      </c>
+      <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>135</v>
-      </c>
+      <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="24"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="39"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="36"/>
+      <c r="Z8" s="36"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="19"/>
-      <c r="I9" s="17" t="s">
-        <v>137</v>
-      </c>
+      <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="24"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
       <c r="S9" s="26"/>
       <c r="T9" s="26"/>
       <c r="U9" s="26"/>
-      <c r="V9" s="40"/>
+      <c r="V9" s="37"/>
       <c r="W9" s="2"/>
       <c r="X9" s="26"/>
       <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="17" t="s">
-        <v>138</v>
-      </c>
+      <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="19"/>
-      <c r="I10" s="17" t="s">
-        <v>139</v>
-      </c>
+      <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
       <c r="U10" s="26"/>
-      <c r="V10" s="40"/>
+      <c r="V10" s="37"/>
       <c r="W10" s="26"/>
       <c r="X10" s="26"/>
       <c r="Y10" s="26"/>
       <c r="Z10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="D11" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="17"/>
       <c r="H11" s="19"/>
-      <c r="I11" s="17" t="s">
-        <v>141</v>
-      </c>
+      <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
-      <c r="L11" s="41"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
+      <c r="L11" s="39"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
       <c r="Q11" s="26"/>
       <c r="R11" s="26"/>
       <c r="S11" s="26"/>
       <c r="T11" s="26"/>
       <c r="U11" s="26"/>
-      <c r="V11" s="40"/>
+      <c r="V11" s="37"/>
       <c r="W11" s="26"/>
-      <c r="X11" s="42"/>
+      <c r="X11" s="40"/>
       <c r="Y11" s="26"/>
-      <c r="Z11" s="42"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z11" s="40"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="17" t="s">
-        <v>142</v>
-      </c>
+      <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="17" t="s">
-        <v>143</v>
-      </c>
+      <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="41"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
+      <c r="L12" s="39"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="26"/>
-      <c r="S12" s="42"/>
+      <c r="S12" s="40"/>
       <c r="T12" s="26"/>
       <c r="U12" s="26"/>
-      <c r="V12" s="40"/>
+      <c r="V12" s="37"/>
       <c r="W12" s="26"/>
       <c r="X12" s="26"/>
       <c r="Y12" s="26"/>
-      <c r="Z12" s="42"/>
+      <c r="Z12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="15" t="s">
@@ -6317,15 +6159,15 @@
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
-      <c r="L13" s="41"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
+      <c r="L13" s="39"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
       <c r="T13" s="26"/>
       <c r="U13" s="26"/>
-      <c r="V13" s="40"/>
+      <c r="V13" s="37"/>
       <c r="W13" s="2"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
@@ -6333,7 +6175,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -6343,16 +6185,16 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="37"/>
+      <c r="K14" s="34"/>
       <c r="L14" s="6"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
       <c r="U14" s="26"/>
-      <c r="V14" s="40"/>
+      <c r="V14" s="37"/>
       <c r="W14" s="26"/>
       <c r="X14" s="26"/>
       <c r="Y14" s="26"/>
@@ -6391,43 +6233,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="15"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="D16" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
       <c r="H16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="17" t="s">
-        <v>146</v>
-      </c>
+      <c r="I16" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="J16" s="17"/>
       <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="15"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
+      <c r="D17" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
       <c r="H17" s="19"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="17" t="s">
-        <v>148</v>
-      </c>
+      <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
     </row>
@@ -6436,17 +6273,13 @@
         <v>20</v>
       </c>
       <c r="C18" s="15"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="17" t="s">
-        <v>149</v>
-      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="19"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="17" t="s">
-        <v>150</v>
-      </c>
+      <c r="J18" s="17"/>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
     </row>
@@ -6455,17 +6288,13 @@
         <v>21</v>
       </c>
       <c r="C19" s="15"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="17" t="s">
-        <v>151</v>
-      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="19"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="17" t="s">
-        <v>152</v>
-      </c>
+      <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
     </row>
@@ -6474,17 +6303,13 @@
         <v>22</v>
       </c>
       <c r="C20" s="15"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="17" t="s">
-        <v>153</v>
-      </c>
+      <c r="D20" s="39"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="19"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="17" t="s">
-        <v>154</v>
-      </c>
+      <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
     </row>
@@ -6493,8 +6318,8 @@
         <v>23</v>
       </c>
       <c r="C21" s="15"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
       <c r="H21" s="19"/>
@@ -6505,7 +6330,7 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -6515,7 +6340,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="37"/>
+      <c r="K22" s="34"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6557,94 +6382,74 @@
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="17" t="s">
-        <v>156</v>
-      </c>
+      <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
       <c r="H24" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="17"/>
-      <c r="J24" s="17" t="s">
-        <v>157</v>
-      </c>
+      <c r="J24" s="17"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="17" t="s">
-        <v>158</v>
-      </c>
+      <c r="E25" s="17"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
       <c r="H25" s="19"/>
       <c r="I25" s="17"/>
-      <c r="J25" s="17" t="s">
-        <v>159</v>
-      </c>
+      <c r="J25" s="17"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="17"/>
-      <c r="E26" s="17" t="s">
-        <v>160</v>
-      </c>
+      <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="19"/>
       <c r="I26" s="17"/>
-      <c r="J26" s="17" t="s">
-        <v>161</v>
-      </c>
+      <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="17" t="s">
-        <v>162</v>
-      </c>
+      <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="19"/>
       <c r="I27" s="17"/>
-      <c r="J27" s="17" t="s">
-        <v>163</v>
-      </c>
+      <c r="J27" s="17"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="17" t="s">
-        <v>164</v>
-      </c>
+      <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="H28" s="19"/>
       <c r="I28" s="17"/>
-      <c r="J28" s="17" t="s">
-        <v>165</v>
-      </c>
+      <c r="J28" s="17"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
     </row>
@@ -6691,7 +6496,7 @@
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="12" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -6701,7 +6506,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="37"/>
+      <c r="K32" s="34"/>
       <c r="L32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6743,7 +6548,7 @@
       </c>
       <c r="C34" s="15"/>
       <c r="E34" s="17" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
@@ -6751,10 +6556,10 @@
         <v>17</v>
       </c>
       <c r="I34" s="17"/>
-      <c r="J34" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="K34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17" t="s">
+        <v>142</v>
+      </c>
       <c r="L34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6769,25 +6574,24 @@
       <c r="H35" s="19"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="15"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="17"/>
       <c r="G36" s="17"/>
       <c r="H36" s="19"/>
       <c r="I36" s="17" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
@@ -6800,14 +6604,14 @@
       <c r="C37" s="15"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
       <c r="H37" s="19"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
@@ -6818,14 +6622,14 @@
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="17" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
       <c r="H38" s="19"/>
       <c r="I38" s="17" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -6848,7 +6652,7 @@
     </row>
     <row r="40" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="12" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -6858,7 +6662,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
-      <c r="K40" s="37"/>
+      <c r="K40" s="34"/>
       <c r="L40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6899,95 +6703,82 @@
         <v>15</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17" t="s">
-        <v>177</v>
-      </c>
+      <c r="D42" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="17"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
       <c r="H42" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17" t="s">
-        <v>179</v>
-      </c>
+      <c r="D43" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
       <c r="H43" s="19"/>
       <c r="I43" s="17"/>
-      <c r="J43" s="17" t="s">
-        <v>180</v>
-      </c>
+      <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17" t="s">
-        <v>181</v>
-      </c>
+      <c r="D44" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
       <c r="H44" s="19"/>
       <c r="I44" s="17"/>
-      <c r="J44" s="17" t="s">
-        <v>182</v>
-      </c>
+      <c r="J44" s="17"/>
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17" t="s">
-        <v>178</v>
-      </c>
+      <c r="D45" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="17"/>
       <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
       <c r="H45" s="19"/>
       <c r="I45" s="17"/>
-      <c r="J45" s="17" t="s">
-        <v>183</v>
-      </c>
+      <c r="J45" s="17"/>
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17" t="s">
-        <v>184</v>
-      </c>
+      <c r="D46" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="17"/>
       <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
       <c r="H46" s="19"/>
       <c r="I46" s="17"/>
-      <c r="J46" s="17" t="s">
-        <v>185</v>
-      </c>
+      <c r="J46" s="17"/>
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
     </row>
@@ -7006,9 +6797,9 @@
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
     </row>
-    <row r="48" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="12" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -7018,7 +6809,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
-      <c r="K48" s="37"/>
+      <c r="K48" s="34"/>
       <c r="L48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7054,14 +6845,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C50" s="15"/>
-      <c r="D50" s="17" t="s">
-        <v>187</v>
-      </c>
+      <c r="D50" s="17"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
@@ -7073,26 +6862,22 @@
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="17" t="s">
-        <v>188</v>
-      </c>
+      <c r="D51" s="17"/>
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
       <c r="H51" s="19"/>
-      <c r="I51" s="17" t="s">
-        <v>189</v>
-      </c>
+      <c r="I51" s="17"/>
       <c r="J51" s="17"/>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="15" t="s">
         <v>20</v>
       </c>
@@ -7107,7 +6892,7 @@
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="15" t="s">
         <v>21</v>
       </c>
@@ -7122,14 +6907,12 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C54" s="15"/>
-      <c r="D54" s="17" t="s">
-        <v>190</v>
-      </c>
+      <c r="D54" s="17"/>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
@@ -7139,16 +6922,14 @@
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C55" s="15"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
-      <c r="F55" s="17" t="s">
-        <v>191</v>
-      </c>
+      <c r="F55" s="17"/>
       <c r="G55" s="17"/>
       <c r="H55" s="19"/>
       <c r="I55" s="17"/>
@@ -7158,7 +6939,7 @@
     </row>
     <row r="57" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="12" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -7168,7 +6949,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-      <c r="K57" s="37"/>
+      <c r="K57" s="34"/>
       <c r="L57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7204,98 +6985,92 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="15"/>
-      <c r="E59" s="17" t="s">
-        <v>193</v>
-      </c>
+      <c r="D59" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" s="17"/>
       <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
       <c r="H59" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="43"/>
-      <c r="J59" s="17" t="s">
-        <v>194</v>
-      </c>
+      <c r="I59" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="J59" s="17"/>
       <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="15"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17" t="s">
-        <v>195</v>
-      </c>
+      <c r="D60" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E60" s="17"/>
       <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
       <c r="H60" s="19"/>
-      <c r="I60" s="43"/>
+      <c r="I60" s="41"/>
       <c r="J60" s="17" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="K60" s="17"/>
       <c r="L60" s="17"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C61" s="15"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17" t="s">
-        <v>197</v>
-      </c>
+      <c r="D61" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E61" s="17"/>
       <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
       <c r="H61" s="19"/>
-      <c r="I61" s="43"/>
+      <c r="I61" s="41"/>
       <c r="J61" s="17" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="K61" s="17"/>
       <c r="L61" s="17"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C62" s="15"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17" t="s">
-        <v>199</v>
-      </c>
+      <c r="D62" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" s="17"/>
       <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
       <c r="H62" s="19"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="17" t="s">
-        <v>200</v>
-      </c>
+      <c r="I62" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="J62" s="17"/>
       <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C63" s="15"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17" t="s">
-        <v>201</v>
-      </c>
+      <c r="D63" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E63" s="17"/>
       <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
       <c r="H63" s="19"/>
-      <c r="I63" s="43"/>
+      <c r="I63" s="41"/>
       <c r="J63" s="17" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="K63" s="17"/>
       <c r="L63" s="17"/>
@@ -7317,7 +7092,7 @@
     </row>
     <row r="66" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="12" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
@@ -7327,7 +7102,7 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
-      <c r="K66" s="37"/>
+      <c r="K66" s="34"/>
       <c r="L66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7363,98 +7138,91 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="15"/>
-      <c r="E68" s="17" t="s">
-        <v>204</v>
-      </c>
+      <c r="D68" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" s="17"/>
       <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
       <c r="H68" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I68" s="43"/>
-      <c r="J68" s="17" t="s">
-        <v>205</v>
-      </c>
+      <c r="I68" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="J68" s="17"/>
       <c r="K68" s="17"/>
-      <c r="L68" s="17"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C69" s="15"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17" t="s">
-        <v>206</v>
-      </c>
+      <c r="D69" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E69" s="17"/>
       <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
       <c r="H69" s="19"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="17" t="s">
-        <v>207</v>
-      </c>
+      <c r="I69" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="J69" s="17"/>
       <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C70" s="15"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17" t="s">
-        <v>208</v>
-      </c>
+      <c r="D70" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="E70" s="17"/>
       <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
       <c r="H70" s="19"/>
-      <c r="I70" s="43"/>
+      <c r="I70" s="41"/>
       <c r="J70" s="17" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
       <c r="K70" s="17"/>
       <c r="L70" s="17"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C71" s="15"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17" t="s">
-        <v>210</v>
-      </c>
+      <c r="D71" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E71" s="17"/>
       <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
       <c r="H71" s="19"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="17" t="s">
-        <v>211</v>
-      </c>
+      <c r="I71" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J71" s="17"/>
       <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C72" s="15"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17" t="s">
-        <v>212</v>
-      </c>
+      <c r="D72" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E72" s="17"/>
       <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
       <c r="H72" s="19"/>
-      <c r="I72" s="43"/>
+      <c r="I72" s="41"/>
       <c r="J72" s="17" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="K72" s="17"/>
       <c r="L72" s="17"/>
@@ -7476,7 +7244,7 @@
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="12" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
@@ -7486,7 +7254,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
-      <c r="K75" s="37"/>
+      <c r="K75" s="34"/>
       <c r="L75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7527,18 +7295,14 @@
         <v>15</v>
       </c>
       <c r="C77" s="15"/>
-      <c r="E77" s="17" t="s">
-        <v>215</v>
-      </c>
+      <c r="E77" s="17"/>
       <c r="F77" s="17"/>
       <c r="G77" s="17"/>
       <c r="H77" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I77" s="17"/>
-      <c r="J77" s="17" t="s">
-        <v>216</v>
-      </c>
+      <c r="J77" s="17"/>
       <c r="K77" s="17"/>
       <c r="L77" s="17"/>
     </row>
@@ -7548,73 +7312,60 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="17"/>
-      <c r="E78" s="17" t="s">
-        <v>217</v>
-      </c>
+      <c r="E78" s="17"/>
       <c r="F78" s="17"/>
       <c r="G78" s="17"/>
       <c r="H78" s="19"/>
       <c r="I78" s="17"/>
-      <c r="J78" s="17" t="s">
-        <v>218</v>
-      </c>
+      <c r="J78" s="17"/>
       <c r="K78" s="17"/>
       <c r="L78" s="17"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C79" s="15"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17" t="s">
-        <v>219</v>
-      </c>
+      <c r="D79" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E79" s="17"/>
       <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
       <c r="H79" s="19"/>
       <c r="I79" s="17"/>
-      <c r="J79" s="17" t="s">
-        <v>220</v>
-      </c>
+      <c r="J79" s="17"/>
       <c r="K79" s="17"/>
       <c r="L79" s="17"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C80" s="15"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17" t="s">
-        <v>221</v>
-      </c>
+      <c r="D80" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E80" s="17"/>
       <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
       <c r="H80" s="19"/>
       <c r="I80" s="17"/>
-      <c r="J80" s="17" t="s">
-        <v>222</v>
-      </c>
+      <c r="J80" s="17"/>
       <c r="K80" s="17"/>
       <c r="L80" s="17"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C81" s="15"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17" t="s">
-        <v>223</v>
-      </c>
+      <c r="D81" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81" s="17"/>
       <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
       <c r="H81" s="19"/>
       <c r="I81" s="17"/>
-      <c r="J81" s="17" t="s">
-        <v>224</v>
-      </c>
+      <c r="J81" s="17"/>
       <c r="K81" s="17"/>
       <c r="L81" s="17"/>
     </row>
@@ -7633,9 +7384,9 @@
       <c r="K82" s="17"/>
       <c r="L82" s="17"/>
     </row>
-    <row r="84" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="12" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
@@ -7645,7 +7396,7 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
-      <c r="K84" s="37"/>
+      <c r="K84" s="34"/>
       <c r="L84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7694,28 +7445,28 @@
         <v>17</v>
       </c>
       <c r="I86" s="17" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="J86" s="17"/>
       <c r="K86" s="17"/>
       <c r="L86" s="17"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C87" s="15"/>
       <c r="D87" s="17"/>
-      <c r="E87" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="F87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="G87" s="17"/>
       <c r="H87" s="19"/>
-      <c r="I87" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="J87" s="17"/>
+      <c r="I87" s="17"/>
+      <c r="J87" s="17" t="s">
+        <v>186</v>
+      </c>
       <c r="K87" s="17"/>
       <c r="L87" s="17"/>
     </row>
@@ -7730,7 +7481,7 @@
       <c r="G88" s="17"/>
       <c r="H88" s="19"/>
       <c r="I88" s="17" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="J88" s="17"/>
       <c r="K88" s="17"/>
@@ -7743,14 +7494,14 @@
       <c r="C89" s="15"/>
       <c r="D89" s="17"/>
       <c r="E89" s="17" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="17"/>
       <c r="H89" s="19"/>
       <c r="I89" s="17"/>
       <c r="J89" s="17" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
@@ -7762,14 +7513,14 @@
       <c r="C90" s="15"/>
       <c r="D90" s="17"/>
       <c r="E90" s="17" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="17"/>
       <c r="H90" s="19"/>
       <c r="I90" s="17"/>
       <c r="J90" s="17" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="K90" s="17"/>
       <c r="L90" s="17"/>
@@ -7815,11 +7566,11 @@
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="D16:F16"/>
     <mergeCell ref="H16:H21"/>
-    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="J17:L17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E18:G18"/>
@@ -7853,11 +7604,11 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="H34:H39"/>
-    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="K34:L34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="E37:F37"/>
@@ -7868,20 +7619,20 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="D42:F42"/>
     <mergeCell ref="H42:H47"/>
     <mergeCell ref="J42:L42"/>
     <mergeCell ref="B43:C43"/>
-    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="D43:F43"/>
     <mergeCell ref="J43:L43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="D44:F44"/>
     <mergeCell ref="J44:L44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="D45:F45"/>
     <mergeCell ref="J45:L45"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="D46:F46"/>
     <mergeCell ref="J46:L46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B49:C49"/>
@@ -7899,38 +7650,38 @@
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="D59:F59"/>
     <mergeCell ref="H59:H64"/>
-    <mergeCell ref="J59:L59"/>
+    <mergeCell ref="I59:K59"/>
     <mergeCell ref="B60:C60"/>
-    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="D60:F60"/>
     <mergeCell ref="J60:L60"/>
     <mergeCell ref="B61:C61"/>
-    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="D61:F61"/>
     <mergeCell ref="J61:L61"/>
     <mergeCell ref="B62:C62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="J62:L62"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="I62:K62"/>
     <mergeCell ref="B63:C63"/>
-    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="D63:F63"/>
     <mergeCell ref="J63:L63"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="D68:F68"/>
     <mergeCell ref="H68:H73"/>
-    <mergeCell ref="J68:L68"/>
+    <mergeCell ref="I68:K68"/>
     <mergeCell ref="B69:C69"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="J69:L69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="I69:K69"/>
     <mergeCell ref="B70:C70"/>
-    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="D70:F70"/>
     <mergeCell ref="J70:L70"/>
     <mergeCell ref="B71:C71"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="J71:L71"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="I71:K71"/>
     <mergeCell ref="B72:C72"/>
-    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="D72:F72"/>
     <mergeCell ref="J72:L72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B76:C76"/>
@@ -7942,13 +7693,13 @@
     <mergeCell ref="E78:G78"/>
     <mergeCell ref="J78:L78"/>
     <mergeCell ref="B79:C79"/>
-    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="D79:F79"/>
     <mergeCell ref="J79:L79"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="D80:F80"/>
     <mergeCell ref="J80:L80"/>
     <mergeCell ref="B81:C81"/>
-    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="D81:F81"/>
     <mergeCell ref="J81:L81"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="B85:C85"/>
@@ -7956,8 +7707,8 @@
     <mergeCell ref="H86:H91"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="B87:C87"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="J87:K87"/>
     <mergeCell ref="B88:C88"/>
     <mergeCell ref="I88:J88"/>
     <mergeCell ref="B89:C89"/>

</xml_diff>